<commit_message>
cap nhat tai lieu bai tap : them noi dung tim kiem
</commit_message>
<xml_diff>
--- a/04.database/mysql.xlsx
+++ b/04.database/mysql.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\hoc_tap\04.database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thaitq\hoc_tap\04.database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng quát" sheetId="8" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="206">
   <si>
     <t>Tạo cơ sở dữ liệu trong MySQL</t>
   </si>
@@ -2411,12 +2411,36 @@
   <si>
     <t>WHERE  manv = 7;</t>
   </si>
+  <si>
+    <t>Năm sinh</t>
+  </si>
+  <si>
+    <t>Tìm kiếm</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Họ tên: Tìm kiếm gần đúng</t>
+  </si>
+  <si>
+    <t>Yêu cầu</t>
+  </si>
+  <si>
+    <t>Năm sinh: Là 1 combobox có sẵn các năm từ 1900 đến năm hiện tại.</t>
+  </si>
+  <si>
+    <t>Số điện thoại: Tương tự họ tên. sau khi nhập giá trị vào input và nhấn tìm kiếm sẽ cho ra kết quả gần đúng</t>
+  </si>
+  <si>
+    <t>Hệ số lương: tìm kiếm hệ số lương nằm trong khoảng.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2563,6 +2587,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2670,7 +2717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2718,15 +2765,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="19" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2755,6 +2793,25 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4355,121 +4412,121 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="30">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="B16" s="27">
+      <c r="B16" s="24">
         <v>1</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="26">
         <v>44107</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="27">
+      <c r="B17" s="24">
         <v>2</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="26">
         <v>44107</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="27">
+      <c r="B18" s="24">
         <v>3</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="26">
         <v>44107</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="27">
+      <c r="B19" s="24">
         <v>4</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="26">
         <v>44107</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="27">
+      <c r="B20" s="24">
         <v>5</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="26">
         <v>44107</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="27">
+      <c r="B21" s="24">
         <v>6</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="26">
         <v>45386</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="27">
         <v>5</v>
       </c>
     </row>
@@ -4479,58 +4536,58 @@
       </c>
     </row>
     <row r="24" spans="2:6" ht="30">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="23" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="25" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="25" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="27" spans="2:6">
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="28" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="28" spans="2:6">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="28" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="28" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="2:6">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="25" t="s">
         <v>146</v>
       </c>
     </row>
@@ -4540,42 +4597,42 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="30">
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="23" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="25" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="25" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="25" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="25" t="s">
         <v>146</v>
       </c>
     </row>
@@ -4599,121 +4656,121 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="30">
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D44" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E44" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F44" s="26" t="s">
+      <c r="F44" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="B45" s="27">
+      <c r="B45" s="24">
         <v>1</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45" s="26">
         <v>44108</v>
       </c>
-      <c r="E45" s="28" t="s">
+      <c r="E45" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F45" s="30">
+      <c r="F45" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="B46" s="27">
+      <c r="B46" s="24">
         <v>2</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D46" s="29">
+      <c r="D46" s="26">
         <v>44109</v>
       </c>
-      <c r="E46" s="28" t="s">
+      <c r="E46" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F46" s="30">
+      <c r="F46" s="27">
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="B47" s="27">
+      <c r="B47" s="24">
         <v>3</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D47" s="29">
+      <c r="D47" s="26">
         <v>44110</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F47" s="30">
+      <c r="F47" s="27">
         <v>2.34</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="B48" s="27">
+      <c r="B48" s="24">
         <v>4</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D48" s="29">
+      <c r="D48" s="26">
         <v>44111</v>
       </c>
-      <c r="E48" s="28" t="s">
+      <c r="E48" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F48" s="30">
+      <c r="F48" s="27">
         <v>2.54</v>
       </c>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="27">
+      <c r="B49" s="24">
         <v>5</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="29">
+      <c r="D49" s="26">
         <v>44112</v>
       </c>
-      <c r="E49" s="28" t="s">
+      <c r="E49" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F49" s="30">
+      <c r="F49" s="27">
         <v>2.44</v>
       </c>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="27">
+      <c r="B50" s="24">
         <v>6</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D50" s="29">
+      <c r="D50" s="26">
         <v>44113</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F50" s="30">
+      <c r="F50" s="27">
         <v>5</v>
       </c>
     </row>
@@ -4723,36 +4780,36 @@
       </c>
     </row>
     <row r="53" spans="2:6" ht="30">
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="26" t="s">
+      <c r="D53" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E53" s="26" t="s">
+      <c r="E53" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F53" s="26" t="s">
+      <c r="F53" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="54" spans="2:6">
-      <c r="B54" s="33">
+      <c r="B54" s="30">
         <v>4</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C54" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D54" s="29">
+      <c r="D54" s="26">
         <v>44111</v>
       </c>
-      <c r="E54" s="28" t="s">
+      <c r="E54" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F54" s="30">
+      <c r="F54" s="27">
         <v>2.54</v>
       </c>
     </row>
@@ -4762,70 +4819,70 @@
       </c>
     </row>
     <row r="57" spans="2:6" ht="30">
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="26" t="s">
+      <c r="D57" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E57" s="26" t="s">
+      <c r="E57" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F57" s="26" t="s">
+      <c r="F57" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="58" spans="2:6">
-      <c r="B58" s="27">
+      <c r="B58" s="24">
         <v>1</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C58" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D58" s="29">
+      <c r="D58" s="26">
         <v>44108</v>
       </c>
-      <c r="E58" s="28" t="s">
+      <c r="E58" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F58" s="34">
+      <c r="F58" s="31">
         <v>2.14</v>
       </c>
     </row>
     <row r="59" spans="2:6">
-      <c r="B59" s="27">
+      <c r="B59" s="24">
         <v>4</v>
       </c>
-      <c r="C59" s="28" t="s">
+      <c r="C59" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D59" s="29">
+      <c r="D59" s="26">
         <v>44111</v>
       </c>
-      <c r="E59" s="28" t="s">
+      <c r="E59" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F59" s="34">
+      <c r="F59" s="31">
         <v>2.54</v>
       </c>
     </row>
     <row r="60" spans="2:6">
-      <c r="B60" s="27">
+      <c r="B60" s="24">
         <v>6</v>
       </c>
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="29">
+      <c r="D60" s="26">
         <v>44113</v>
       </c>
-      <c r="E60" s="28" t="s">
+      <c r="E60" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F60" s="34">
+      <c r="F60" s="31">
         <v>5</v>
       </c>
     </row>
@@ -4835,53 +4892,53 @@
       </c>
     </row>
     <row r="63" spans="2:6" ht="30">
-      <c r="B63" s="26" t="s">
+      <c r="B63" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="C63" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D63" s="26" t="s">
+      <c r="D63" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="26" t="s">
+      <c r="E63" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F63" s="26" t="s">
+      <c r="F63" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="64" spans="2:6">
-      <c r="B64" s="27">
+      <c r="B64" s="24">
         <v>5</v>
       </c>
-      <c r="C64" s="28" t="s">
+      <c r="C64" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D64" s="35">
+      <c r="D64" s="32">
         <v>44112</v>
       </c>
-      <c r="E64" s="28" t="s">
+      <c r="E64" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F64" s="34">
+      <c r="F64" s="31">
         <v>2.44</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="B65" s="27">
+      <c r="B65" s="24">
         <v>6</v>
       </c>
-      <c r="C65" s="28" t="s">
+      <c r="C65" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D65" s="35">
+      <c r="D65" s="32">
         <v>44113</v>
       </c>
-      <c r="E65" s="28" t="s">
+      <c r="E65" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F65" s="34">
+      <c r="F65" s="31">
         <v>5</v>
       </c>
     </row>
@@ -4896,7 +4953,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75">
-      <c r="B71" s="32" t="s">
+      <c r="B71" s="29" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4906,121 +4963,121 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="30">
-      <c r="B74" s="26" t="s">
+      <c r="B74" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C74" s="26" t="s">
+      <c r="C74" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D74" s="26" t="s">
+      <c r="D74" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E74" s="26" t="s">
+      <c r="E74" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F74" s="26" t="s">
+      <c r="F74" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="B75" s="33">
+      <c r="B75" s="30">
         <v>6</v>
       </c>
-      <c r="C75" s="28" t="s">
+      <c r="C75" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D75" s="29">
+      <c r="D75" s="26">
         <v>44113</v>
       </c>
-      <c r="E75" s="28" t="s">
+      <c r="E75" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F75" s="30">
+      <c r="F75" s="27">
         <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="B76" s="33">
+      <c r="B76" s="30">
         <v>5</v>
       </c>
-      <c r="C76" s="28" t="s">
+      <c r="C76" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D76" s="29">
+      <c r="D76" s="26">
         <v>44112</v>
       </c>
-      <c r="E76" s="28" t="s">
+      <c r="E76" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F76" s="30">
+      <c r="F76" s="27">
         <v>2.44</v>
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="B77" s="33">
+      <c r="B77" s="30">
         <v>4</v>
       </c>
-      <c r="C77" s="28" t="s">
+      <c r="C77" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D77" s="29">
+      <c r="D77" s="26">
         <v>44111</v>
       </c>
-      <c r="E77" s="28" t="s">
+      <c r="E77" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F77" s="30">
+      <c r="F77" s="27">
         <v>2.54</v>
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="B78" s="33">
+      <c r="B78" s="30">
         <v>3</v>
       </c>
-      <c r="C78" s="28" t="s">
+      <c r="C78" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D78" s="29">
+      <c r="D78" s="26">
         <v>44110</v>
       </c>
-      <c r="E78" s="28" t="s">
+      <c r="E78" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F78" s="30">
+      <c r="F78" s="27">
         <v>2.34</v>
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="B79" s="33">
+      <c r="B79" s="30">
         <v>2</v>
       </c>
-      <c r="C79" s="28" t="s">
+      <c r="C79" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D79" s="29">
+      <c r="D79" s="26">
         <v>44109</v>
       </c>
-      <c r="E79" s="28" t="s">
+      <c r="E79" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F79" s="30">
+      <c r="F79" s="27">
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="B80" s="33">
+      <c r="B80" s="30">
         <v>1</v>
       </c>
-      <c r="C80" s="28" t="s">
+      <c r="C80" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D80" s="29">
+      <c r="D80" s="26">
         <v>44108</v>
       </c>
-      <c r="E80" s="28" t="s">
+      <c r="E80" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F80" s="30">
+      <c r="F80" s="27">
         <v>2.14</v>
       </c>
     </row>
@@ -5030,121 +5087,121 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="30">
-      <c r="B83" s="26" t="s">
+      <c r="B83" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C83" s="26" t="s">
+      <c r="C83" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D83" s="26" t="s">
+      <c r="D83" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E83" s="26" t="s">
+      <c r="E83" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F83" s="26" t="s">
+      <c r="F83" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="B84" s="27">
+      <c r="B84" s="24">
         <v>1</v>
       </c>
-      <c r="C84" s="28" t="s">
+      <c r="C84" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D84" s="29">
+      <c r="D84" s="26">
         <v>44108</v>
       </c>
-      <c r="E84" s="31" t="s">
+      <c r="E84" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="F84" s="34">
+      <c r="F84" s="31">
         <v>2.14</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="B85" s="27">
+      <c r="B85" s="24">
         <v>2</v>
       </c>
-      <c r="C85" s="28" t="s">
+      <c r="C85" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D85" s="29">
+      <c r="D85" s="26">
         <v>44109</v>
       </c>
-      <c r="E85" s="31" t="s">
+      <c r="E85" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="F85" s="34">
+      <c r="F85" s="31">
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="B86" s="27">
+      <c r="B86" s="24">
         <v>3</v>
       </c>
-      <c r="C86" s="28" t="s">
+      <c r="C86" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D86" s="29">
+      <c r="D86" s="26">
         <v>44110</v>
       </c>
-      <c r="E86" s="31" t="s">
+      <c r="E86" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="F86" s="34">
+      <c r="F86" s="31">
         <v>2.34</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="B87" s="27">
+      <c r="B87" s="24">
         <v>5</v>
       </c>
-      <c r="C87" s="28" t="s">
+      <c r="C87" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D87" s="29">
+      <c r="D87" s="26">
         <v>44112</v>
       </c>
-      <c r="E87" s="31" t="s">
+      <c r="E87" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="F87" s="34">
+      <c r="F87" s="31">
         <v>2.44</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="B88" s="27">
+      <c r="B88" s="24">
         <v>4</v>
       </c>
-      <c r="C88" s="28" t="s">
+      <c r="C88" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D88" s="29">
+      <c r="D88" s="26">
         <v>44111</v>
       </c>
-      <c r="E88" s="31" t="s">
+      <c r="E88" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="F88" s="34">
+      <c r="F88" s="31">
         <v>2.54</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="B89" s="27">
+      <c r="B89" s="24">
         <v>6</v>
       </c>
-      <c r="C89" s="28" t="s">
+      <c r="C89" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D89" s="29">
+      <c r="D89" s="26">
         <v>44113</v>
       </c>
-      <c r="E89" s="31" t="s">
+      <c r="E89" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="F89" s="34">
+      <c r="F89" s="31">
         <v>5</v>
       </c>
     </row>
@@ -5154,7 +5211,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75">
-      <c r="B92" s="32" t="s">
+      <c r="B92" s="29" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5164,121 +5221,121 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="30">
-      <c r="B94" s="26" t="s">
+      <c r="B94" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C94" s="26" t="s">
+      <c r="C94" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D94" s="26" t="s">
+      <c r="D94" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E94" s="26" t="s">
+      <c r="E94" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F94" s="26" t="s">
+      <c r="F94" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="B95" s="27">
+      <c r="B95" s="24">
         <v>1</v>
       </c>
-      <c r="C95" s="28" t="s">
+      <c r="C95" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D95" s="29">
+      <c r="D95" s="26">
         <v>44108</v>
       </c>
-      <c r="E95" s="28" t="s">
+      <c r="E95" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F95" s="30">
+      <c r="F95" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="B96" s="27">
+      <c r="B96" s="24">
         <v>2</v>
       </c>
-      <c r="C96" s="28" t="s">
+      <c r="C96" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D96" s="29">
+      <c r="D96" s="26">
         <v>44109</v>
       </c>
-      <c r="E96" s="28" t="s">
+      <c r="E96" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F96" s="30">
+      <c r="F96" s="27">
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="97" spans="2:6">
-      <c r="B97" s="27">
+      <c r="B97" s="24">
         <v>3</v>
       </c>
-      <c r="C97" s="28" t="s">
+      <c r="C97" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D97" s="29">
+      <c r="D97" s="26">
         <v>44110</v>
       </c>
-      <c r="E97" s="28" t="s">
+      <c r="E97" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F97" s="30">
+      <c r="F97" s="27">
         <v>2.34</v>
       </c>
     </row>
     <row r="98" spans="2:6">
-      <c r="B98" s="27">
+      <c r="B98" s="24">
         <v>4</v>
       </c>
-      <c r="C98" s="28" t="s">
+      <c r="C98" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D98" s="29">
+      <c r="D98" s="26">
         <v>44111</v>
       </c>
-      <c r="E98" s="28" t="s">
+      <c r="E98" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F98" s="30">
+      <c r="F98" s="27">
         <v>2.54</v>
       </c>
     </row>
     <row r="99" spans="2:6">
-      <c r="B99" s="27">
+      <c r="B99" s="24">
         <v>5</v>
       </c>
-      <c r="C99" s="28" t="s">
+      <c r="C99" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D99" s="29">
+      <c r="D99" s="26">
         <v>44112</v>
       </c>
-      <c r="E99" s="28" t="s">
+      <c r="E99" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F99" s="30">
+      <c r="F99" s="27">
         <v>2.44</v>
       </c>
     </row>
     <row r="100" spans="2:6">
-      <c r="B100" s="27">
+      <c r="B100" s="24">
         <v>6</v>
       </c>
-      <c r="C100" s="28" t="s">
+      <c r="C100" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D100" s="29">
+      <c r="D100" s="26">
         <v>44113</v>
       </c>
-      <c r="E100" s="28" t="s">
+      <c r="E100" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F100" s="30">
+      <c r="F100" s="27">
         <v>5</v>
       </c>
     </row>
@@ -5288,87 +5345,87 @@
       </c>
     </row>
     <row r="103" spans="2:6" ht="30">
-      <c r="B103" s="26" t="s">
+      <c r="B103" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C103" s="26" t="s">
+      <c r="C103" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D103" s="26" t="s">
+      <c r="D103" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E103" s="26" t="s">
+      <c r="E103" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F103" s="26" t="s">
+      <c r="F103" s="23" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="104" spans="2:6">
-      <c r="B104" s="27">
+      <c r="B104" s="24">
         <v>1</v>
       </c>
-      <c r="C104" s="28" t="s">
+      <c r="C104" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="D104" s="29">
+      <c r="D104" s="26">
         <v>44108</v>
       </c>
-      <c r="E104" s="28" t="s">
+      <c r="E104" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F104" s="30">
+      <c r="F104" s="27">
         <v>2.14</v>
       </c>
     </row>
     <row r="105" spans="2:6">
-      <c r="B105" s="27">
+      <c r="B105" s="24">
         <v>2</v>
       </c>
-      <c r="C105" s="28" t="s">
+      <c r="C105" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="D105" s="29">
+      <c r="D105" s="26">
         <v>44109</v>
       </c>
-      <c r="E105" s="28" t="s">
+      <c r="E105" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F105" s="30">
+      <c r="F105" s="27">
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="106" spans="2:6">
-      <c r="B106" s="27">
+      <c r="B106" s="24">
         <v>3</v>
       </c>
-      <c r="C106" s="28" t="s">
+      <c r="C106" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D106" s="29">
+      <c r="D106" s="26">
         <v>44110</v>
       </c>
-      <c r="E106" s="28" t="s">
+      <c r="E106" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F106" s="30">
+      <c r="F106" s="27">
         <v>2.34</v>
       </c>
     </row>
     <row r="107" spans="2:6">
-      <c r="B107" s="27">
+      <c r="B107" s="24">
         <v>5</v>
       </c>
-      <c r="C107" s="28" t="s">
+      <c r="C107" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="D107" s="29">
+      <c r="D107" s="26">
         <v>44112</v>
       </c>
-      <c r="E107" s="28" t="s">
+      <c r="E107" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F107" s="30">
+      <c r="F107" s="27">
         <v>2.44</v>
       </c>
     </row>
@@ -5478,7 +5535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9:C11"/>
     </sheetView>
   </sheetViews>
@@ -5495,7 +5552,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>185</v>
       </c>
     </row>
@@ -5555,7 +5612,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>194</v>
       </c>
     </row>
@@ -5726,11 +5783,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H38"/>
+  <dimension ref="B1:K50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5741,262 +5796,331 @@
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="2:11">
       <c r="B1" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:11">
       <c r="B2" s="1"/>
-      <c r="H2" s="20" t="s">
+      <c r="K2" s="41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
+      <c r="K3" s="41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="K4" s="41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="K5" s="41" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="K6" s="41" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="9" spans="2:11" ht="15.75">
+      <c r="B9" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="37"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="1"/>
+      <c r="E11" s="36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="1"/>
+      <c r="H12" s="20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
-      <c r="B3" s="19" t="s">
+    <row r="13" spans="2:11">
+      <c r="B13" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C13" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D13" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F13" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G13" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="18">
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C14" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D14" s="17">
         <v>44107</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E14" s="16">
         <v>1111</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F14" s="16">
         <v>1.2</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G14" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H14" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="18">
+    <row r="15" spans="2:11">
+      <c r="B15" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D15" s="17">
         <v>44107</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E15" s="16">
         <v>1111</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F15" s="16">
         <v>1.2</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G15" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H15" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="18">
+    <row r="16" spans="2:11">
+      <c r="B16" s="18">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D16" s="17">
         <v>44107</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E16" s="16">
         <v>1111</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F16" s="16">
         <v>1.2</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G16" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H16" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="18">
+    <row r="17" spans="2:8">
+      <c r="B17" s="18">
         <v>4</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D17" s="17">
         <v>44107</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E17" s="16">
         <v>1111</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F17" s="16">
         <v>1.2</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G17" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H17" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="18">
+    <row r="18" spans="2:8">
+      <c r="B18" s="18">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C18" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D18" s="17">
         <v>44107</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E18" s="16">
         <v>1111</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F18" s="16">
         <v>1.2</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G18" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H18" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="1" t="s">
+    <row r="22" spans="2:8">
+      <c r="B22" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
-      <c r="C11" t="s">
+    <row r="23" spans="2:8">
+      <c r="C23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="C14" t="s">
+    <row r="24" spans="2:8">
+      <c r="C24" s="34"/>
+      <c r="D24" s="35"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="C26" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="C17" t="s">
+    <row r="27" spans="2:8">
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="C29" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="C20" t="s">
+    <row r="30" spans="2:8">
+      <c r="C30" s="34"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="C32" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="C23" s="21" t="s">
+    <row r="33" spans="2:4">
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="C35" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D35" s="22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="1" t="s">
+    <row r="37" spans="2:4">
+      <c r="B37" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
-      <c r="C26" t="s">
+    <row r="38" spans="2:4">
+      <c r="C38" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
-      <c r="C27" s="23"/>
-      <c r="D27" s="24"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="C29" t="s">
+    <row r="39" spans="2:4">
+      <c r="C39" s="34"/>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="C41" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="C32" t="s">
+    <row r="42" spans="2:4">
+      <c r="C42" s="34"/>
+      <c r="D42" s="35"/>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="C44" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-    </row>
-    <row r="35" spans="3:4">
-      <c r="C35" t="s">
+    <row r="45" spans="2:4">
+      <c r="C45" s="34"/>
+      <c r="D45" s="35"/>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="C47" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="3:4">
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-    </row>
-    <row r="38" spans="3:4">
-      <c r="C38" s="21" t="s">
+    <row r="48" spans="2:4">
+      <c r="C48" s="34"/>
+      <c r="D48" s="35"/>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D50" s="22" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C21:D21"/>
+  <mergeCells count="10">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C48:D48"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>